<commit_message>
New changes as part of Excel logic and new tests
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData.xlsx
+++ b/src/test/resources/testData/TestData.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data Drive\Automation\SeleniumAutomation\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1A154AB-9A45-4E89-B52C-571932D0DCC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFACD858-EE12-4957-B535-82412E0737C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -39,9 +39,6 @@
     <t>last_name</t>
   </si>
   <si>
-    <t>dob</t>
-  </si>
-  <si>
     <t>address</t>
   </si>
   <si>
@@ -57,9 +54,6 @@
     <t>country</t>
   </si>
   <si>
-    <t>email</t>
-  </si>
-  <si>
     <t>password</t>
   </si>
   <si>
@@ -81,22 +75,50 @@
     <t>India</t>
   </si>
   <si>
-    <t>test@gmail.com</t>
-  </si>
-  <si>
-    <t>Testing@1234</t>
-  </si>
-  <si>
     <t>695011</t>
   </si>
   <si>
-    <t>07/22/1990</t>
+    <t>year</t>
+  </si>
+  <si>
+    <t>day</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>1990</t>
+  </si>
+  <si>
+    <t>07</t>
+  </si>
+  <si>
+    <t>loginTest</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>month</t>
+  </si>
+  <si>
+    <t>ky25l8apte@gmail.com</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>TestDemo@1234</t>
+  </si>
+  <si>
+    <t>gahzypjin9@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -420,91 +442,146 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="9.453125"/>
+    <col min="5" max="6" customWidth="true" width="9.453125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="E1" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="F1" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="G1" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="M1" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="J1" t="s">
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A2" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="K1" t="s">
+      <c r="C2" t="s" s="0">
         <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" t="s">
-        <v>13</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E2" t="s">
-        <v>14</v>
+      <c r="E2" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="J2" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="K2" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="H2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>19</v>
+      <c r="L2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A3" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="F3" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="G3" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="H3" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="I3" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="J3" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="K3" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="L3" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J2" r:id="rId1" xr:uid="{992C9E80-D11D-4717-A1E9-CA976C160419}"/>
-    <hyperlink ref="K2" r:id="rId2" xr:uid="{8BF9383B-508C-495F-95C2-4AF16E8EED94}"/>
+    <hyperlink ref="L2" r:id="rId1" xr:uid="{992C9E80-D11D-4717-A1E9-CA976C160419}"/>
+    <hyperlink ref="M2" r:id="rId2" xr:uid="{8BF9383B-508C-495F-95C2-4AF16E8EED94}"/>
+    <hyperlink ref="M3" r:id="rId3" xr:uid="{B7569F1B-7382-4FCA-9465-5F8DB5C1B85F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Changes as part of allure reporting
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData.xlsx
+++ b/src/test/resources/testData/TestData.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="52">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -112,6 +112,75 @@
   </si>
   <si>
     <t>gahzypjin9@gmail.com</t>
+  </si>
+  <si>
+    <t>0xojn3ba6m@gmail.com</t>
+  </si>
+  <si>
+    <t>enxhtgagmf@gmail.com</t>
+  </si>
+  <si>
+    <t>6p6glj47rk@gmail.com</t>
+  </si>
+  <si>
+    <t>f6xp5vzc1r@gmail.com</t>
+  </si>
+  <si>
+    <t>1wk9duo5qw@gmail.com</t>
+  </si>
+  <si>
+    <t>xhxc6ven8m@gmail.com</t>
+  </si>
+  <si>
+    <t>dzartll2by@gmail.com</t>
+  </si>
+  <si>
+    <t>boytuvpfrt@gmail.com</t>
+  </si>
+  <si>
+    <t>etrihexxvs@gmail.com</t>
+  </si>
+  <si>
+    <t>v3vtt0rdsw@gmail.com</t>
+  </si>
+  <si>
+    <t>veolxpzlgb@gmail.com</t>
+  </si>
+  <si>
+    <t>svgojyhwj5@gmail.com</t>
+  </si>
+  <si>
+    <t>jp3sdmmizx@gmail.com</t>
+  </si>
+  <si>
+    <t>xomxvldlbg@gmail.com</t>
+  </si>
+  <si>
+    <t>9lwtjx1d1x@gmail.com</t>
+  </si>
+  <si>
+    <t>izweqaoaqb@gmail.com</t>
+  </si>
+  <si>
+    <t>uz05c9dlbk@gmail.com</t>
+  </si>
+  <si>
+    <t>lhpsdvljsv@gmail.com</t>
+  </si>
+  <si>
+    <t>gikjotnlnb@gmail.com</t>
+  </si>
+  <si>
+    <t>67n9yvixlk@gmail.com</t>
+  </si>
+  <si>
+    <t>wp7zksombi@gmail.com</t>
+  </si>
+  <si>
+    <t>yv7gnn7jxq@gmail.com</t>
+  </si>
+  <si>
+    <t>bne0utiuzq@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -530,7 +599,7 @@
         <v>15</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>27</v>
@@ -571,7 +640,7 @@
         <v>23</v>
       </c>
       <c r="L3" t="s" s="0">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="M3" s="1" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
Optimized driver factory and selenium grid implementation
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData.xlsx
+++ b/src/test/resources/testData/TestData.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="43">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -148,6 +148,12 @@
   </si>
   <si>
     <t>lnm9raaifw@gmail.com</t>
+  </si>
+  <si>
+    <t>g0rhiymkzq@gmail.com</t>
+  </si>
+  <si>
+    <t>xecz6lgnck@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -566,7 +572,7 @@
         <v>15</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>26</v>
@@ -607,7 +613,7 @@
         <v>23</v>
       </c>
       <c r="L3" t="s" s="0">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="M3" s="1" t="s">
         <v>26</v>

</xml_diff>